<commit_message>
Update template Excel files for course and schedule management
</commit_message>
<xml_diff>
--- a/public/template/file/mau_ct_dao_tao.xlsx
+++ b/public/template/file/mau_ct_dao_tao.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huuduc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tkb-ptit-react\public\template\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A601C85-E97B-466C-83F7-E8D2E15A35CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D902D6A-8837-43CD-9D60-BA589CDA7383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{080283F8-8324-4DC5-93B8-D8776733EF20}"/>
   </bookViews>
@@ -38,8 +38,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Minh GV</author>
+  </authors>
+  <commentList>
+    <comment ref="K15" authorId="0" shapeId="0" xr:uid="{B34F9399-8FBF-441D-94FB-20EEABD70A45}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Minh GV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Bộ môn chọn ngày 26/2/2025</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="85">
   <si>
     <t>MMH</t>
   </si>
@@ -102,13 +136,205 @@
   </si>
   <si>
     <t>Môn chung</t>
+  </si>
+  <si>
+    <t>SKD1108</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>Phương pháp luận nghiên cứu khoa học</t>
+  </si>
+  <si>
+    <t>VKT</t>
+  </si>
+  <si>
+    <t>Kỹ năng mềm</t>
+  </si>
+  <si>
+    <t>Bài tập lớn</t>
+  </si>
+  <si>
+    <t>INT1482</t>
+  </si>
+  <si>
+    <t>An toàn mạng</t>
+  </si>
+  <si>
+    <t>AT1</t>
+  </si>
+  <si>
+    <t>An toàn thông tin</t>
+  </si>
+  <si>
+    <t>MT:INT1472</t>
+  </si>
+  <si>
+    <t>Thực hành (Phòng máy)</t>
+  </si>
+  <si>
+    <t>INT14105</t>
+  </si>
+  <si>
+    <t>An toàn ứng dụng web và cơ sở dữ liệu</t>
+  </si>
+  <si>
+    <t>Trắc nghiệm (Trên máy)</t>
+  </si>
+  <si>
+    <t>INT1342M</t>
+  </si>
+  <si>
+    <t>Phân tích và thiết kế hệ thống thông tin</t>
+  </si>
+  <si>
+    <t>CN1</t>
+  </si>
+  <si>
+    <t>Công nghệ phần mềm</t>
+  </si>
+  <si>
+    <t>INT14149</t>
+  </si>
+  <si>
+    <t>IoT và ứng dụng</t>
+  </si>
+  <si>
+    <t>Hệ thống thông tin</t>
+  </si>
+  <si>
+    <t>INT1434</t>
+  </si>
+  <si>
+    <t>Lập trình Web</t>
+  </si>
+  <si>
+    <t>MT:INT1339</t>
+  </si>
+  <si>
+    <t>INT14164</t>
+  </si>
+  <si>
+    <t>Phân tích mã độc</t>
+  </si>
+  <si>
+    <t>Phòng máy</t>
+  </si>
+  <si>
+    <t>MUL14188</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>Dẫn chương trình</t>
+  </si>
+  <si>
+    <t>PT1</t>
+  </si>
+  <si>
+    <t>Báo chí</t>
+  </si>
+  <si>
+    <t>Viết</t>
+  </si>
+  <si>
+    <t>MUL14189</t>
+  </si>
+  <si>
+    <t>Vận hành toà soạn báo chí số</t>
+  </si>
+  <si>
+    <t>MUL14194</t>
+  </si>
+  <si>
+    <t>Công nghệ AI trong phân tích dữ liệu báo chí số</t>
+  </si>
+  <si>
+    <t>MUL14185</t>
+  </si>
+  <si>
+    <t>Báo chí và dư luận xã hội</t>
+  </si>
+  <si>
+    <t>MUL14184</t>
+  </si>
+  <si>
+    <t>Báo chí đương đại</t>
+  </si>
+  <si>
+    <t>MUL14197</t>
+  </si>
+  <si>
+    <t>Quảng cáo trên báo chí số</t>
+  </si>
+  <si>
+    <t>MUL1422</t>
+  </si>
+  <si>
+    <t>Tổ chức sản xuất sản phẩm đa phương tiện</t>
+  </si>
+  <si>
+    <t>MUL14199</t>
+  </si>
+  <si>
+    <t>Công nghệ mô phỏng trong báo chí số</t>
+  </si>
+  <si>
+    <t>BAS1160</t>
+  </si>
+  <si>
+    <t>Tiếng Anh (Course 3 Plus)</t>
+  </si>
+  <si>
+    <t>CB1</t>
+  </si>
+  <si>
+    <t>Ngoại ngữ</t>
+  </si>
+  <si>
+    <t>MT:BAS1159</t>
+  </si>
+  <si>
+    <t>Tự luận+Vấn đáp</t>
+  </si>
+  <si>
+    <t>Chung</t>
+  </si>
+  <si>
+    <t>BAS1153</t>
+  </si>
+  <si>
+    <t>ACCA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      Lịch sử Đảng cộng sản Việt Nam</t>
+  </si>
+  <si>
+    <t>Mác - Lê</t>
+  </si>
+  <si>
+    <t>MT:BAS1122</t>
+  </si>
+  <si>
+    <t>Lịch sử Đảng cộng sản Việt Nam</t>
+  </si>
+  <si>
+    <t>SKD1102</t>
+  </si>
+  <si>
+    <t>Kỹ năng làm việc nhóm</t>
+  </si>
+  <si>
+    <t>CN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +353,37 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -155,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -171,6 +428,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,11 +780,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DE5E36-27AA-4A14-8D91-698733F7987A}">
-  <dimension ref="A1:Y2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DE5E36-27AA-4A14-8D91-698733F7987A}">
+  <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,8 +917,1351 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="5"/>
     </row>
+    <row r="3" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="7">
+        <v>211</v>
+      </c>
+      <c r="H3" s="7">
+        <v>4</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="6">
+        <v>2</v>
+      </c>
+      <c r="L3" s="6">
+        <v>30</v>
+      </c>
+      <c r="M3" s="6">
+        <v>18</v>
+      </c>
+      <c r="N3" s="6">
+        <v>6</v>
+      </c>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6">
+        <v>6</v>
+      </c>
+      <c r="R3" s="7"/>
+      <c r="S3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="U3" s="7"/>
+      <c r="V3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X3" s="2"/>
+    </row>
+    <row r="4" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="7">
+        <v>211</v>
+      </c>
+      <c r="H4" s="7">
+        <v>4</v>
+      </c>
+      <c r="I4" s="7"/>
+      <c r="J4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="6">
+        <v>3</v>
+      </c>
+      <c r="L4" s="6">
+        <v>45</v>
+      </c>
+      <c r="M4" s="6">
+        <v>30</v>
+      </c>
+      <c r="N4" s="6">
+        <v>2</v>
+      </c>
+      <c r="O4" s="6">
+        <v>6</v>
+      </c>
+      <c r="P4" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>1</v>
+      </c>
+      <c r="R4" s="7"/>
+      <c r="S4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="7">
+        <v>211</v>
+      </c>
+      <c r="H5" s="7">
+        <v>4</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="6">
+        <v>3</v>
+      </c>
+      <c r="L5" s="6">
+        <v>45</v>
+      </c>
+      <c r="M5" s="6">
+        <v>30</v>
+      </c>
+      <c r="N5" s="6">
+        <v>2</v>
+      </c>
+      <c r="O5" s="6">
+        <v>6</v>
+      </c>
+      <c r="P5" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>1</v>
+      </c>
+      <c r="R5" s="7"/>
+      <c r="S5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X5" s="2"/>
+    </row>
+    <row r="6" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="7">
+        <v>211</v>
+      </c>
+      <c r="H6" s="7">
+        <v>4</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="6">
+        <v>3</v>
+      </c>
+      <c r="L6" s="6">
+        <v>45</v>
+      </c>
+      <c r="M6" s="6">
+        <v>36</v>
+      </c>
+      <c r="N6" s="6">
+        <v>8</v>
+      </c>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="7"/>
+      <c r="S6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" s="7"/>
+      <c r="V6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="X6" s="2"/>
+    </row>
+    <row r="7" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="7">
+        <v>211</v>
+      </c>
+      <c r="H7" s="7">
+        <v>4</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="6">
+        <v>3</v>
+      </c>
+      <c r="L7" s="6">
+        <v>45</v>
+      </c>
+      <c r="M7" s="6">
+        <v>30</v>
+      </c>
+      <c r="N7" s="6">
+        <v>8</v>
+      </c>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>1</v>
+      </c>
+      <c r="R7" s="7"/>
+      <c r="S7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X7" s="2"/>
+    </row>
+    <row r="8" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="7">
+        <v>211</v>
+      </c>
+      <c r="H8" s="7">
+        <v>4</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="6">
+        <v>3</v>
+      </c>
+      <c r="L8" s="6">
+        <v>45</v>
+      </c>
+      <c r="M8" s="6">
+        <v>30</v>
+      </c>
+      <c r="N8" s="6">
+        <v>8</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>1</v>
+      </c>
+      <c r="R8" s="7"/>
+      <c r="S8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="U8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="X8" s="2"/>
+    </row>
+    <row r="9" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="7">
+        <v>211</v>
+      </c>
+      <c r="H9" s="7">
+        <v>4</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="9">
+        <v>2</v>
+      </c>
+      <c r="L9" s="9">
+        <v>30</v>
+      </c>
+      <c r="M9" s="9">
+        <v>12</v>
+      </c>
+      <c r="N9" s="9">
+        <v>14</v>
+      </c>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="W9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="X9" s="2"/>
+    </row>
+    <row r="10" spans="1:25" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="6">
+        <v>63</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="6">
+        <v>2</v>
+      </c>
+      <c r="L10" s="6">
+        <v>30</v>
+      </c>
+      <c r="M10" s="6">
+        <v>15</v>
+      </c>
+      <c r="N10" s="6">
+        <v>15</v>
+      </c>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="X10" s="6"/>
+    </row>
+    <row r="11" spans="1:25" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="6">
+        <v>63</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="6">
+        <v>2</v>
+      </c>
+      <c r="L11" s="6">
+        <v>30</v>
+      </c>
+      <c r="M11" s="6">
+        <v>15</v>
+      </c>
+      <c r="N11" s="6">
+        <v>15</v>
+      </c>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="W11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="X11" s="6"/>
+    </row>
+    <row r="12" spans="1:25" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="6">
+        <v>63</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="6">
+        <v>3</v>
+      </c>
+      <c r="L12" s="6">
+        <v>45</v>
+      </c>
+      <c r="M12" s="6">
+        <v>34</v>
+      </c>
+      <c r="N12" s="6">
+        <v>10</v>
+      </c>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6">
+        <v>1</v>
+      </c>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="X12" s="6"/>
+    </row>
+    <row r="13" spans="1:25" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="6">
+        <v>63</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" s="6">
+        <v>2</v>
+      </c>
+      <c r="L13" s="6">
+        <v>30</v>
+      </c>
+      <c r="M13" s="6">
+        <v>24</v>
+      </c>
+      <c r="N13" s="6">
+        <v>6</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="T13" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="X13" s="6"/>
+    </row>
+    <row r="14" spans="1:25" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="7">
+        <v>2022</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="6">
+        <v>63</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1</v>
+      </c>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" s="6">
+        <v>2</v>
+      </c>
+      <c r="L14" s="6">
+        <v>30</v>
+      </c>
+      <c r="M14" s="6">
+        <v>24</v>
+      </c>
+      <c r="N14" s="6">
+        <v>6</v>
+      </c>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="T14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="W14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="X14" s="6"/>
+    </row>
+    <row r="15" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="10">
+        <v>2022</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="6">
+        <v>63</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6"/>
+      <c r="J15" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K15" s="9">
+        <v>2</v>
+      </c>
+      <c r="L15" s="9">
+        <v>30</v>
+      </c>
+      <c r="M15" s="9">
+        <v>24</v>
+      </c>
+      <c r="N15" s="9">
+        <v>6</v>
+      </c>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="T15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="X15" s="9"/>
+    </row>
+    <row r="16" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="10">
+        <v>2022</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="6">
+        <v>63</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" s="9">
+        <v>2</v>
+      </c>
+      <c r="L16" s="9">
+        <v>30</v>
+      </c>
+      <c r="M16" s="9">
+        <v>24</v>
+      </c>
+      <c r="N16" s="9">
+        <v>6</v>
+      </c>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="T16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="W16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="X16" s="9"/>
+    </row>
+    <row r="17" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="10">
+        <v>2022</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="6">
+        <v>63</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" s="9">
+        <v>2</v>
+      </c>
+      <c r="L17" s="9">
+        <v>30</v>
+      </c>
+      <c r="M17" s="9">
+        <v>24</v>
+      </c>
+      <c r="N17" s="9">
+        <v>6</v>
+      </c>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="T17" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="W17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="X17" s="9"/>
+    </row>
+    <row r="18" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="2">
+        <v>244</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K18" s="6">
+        <v>2</v>
+      </c>
+      <c r="L18" s="6">
+        <v>30</v>
+      </c>
+      <c r="M18" s="6">
+        <v>30</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="U18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="V18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="W18" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="2">
+        <v>26</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="K19" s="6">
+        <v>2</v>
+      </c>
+      <c r="L19" s="6">
+        <v>30</v>
+      </c>
+      <c r="M19" s="6">
+        <v>24</v>
+      </c>
+      <c r="N19" s="6">
+        <v>6</v>
+      </c>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T19" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="U19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="V19" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="W19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="2">
+        <v>244</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="6">
+        <v>2</v>
+      </c>
+      <c r="L20" s="6">
+        <v>30</v>
+      </c>
+      <c r="M20" s="6">
+        <v>24</v>
+      </c>
+      <c r="N20" s="6">
+        <v>6</v>
+      </c>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T20" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="U20" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="V20" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="W20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="2">
+        <v>67</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" s="6">
+        <v>2</v>
+      </c>
+      <c r="L21" s="6">
+        <v>30</v>
+      </c>
+      <c r="M21" s="6">
+        <v>30</v>
+      </c>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="U21" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="V21" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="W21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="2">
+        <v>67</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" s="6">
+        <v>1</v>
+      </c>
+      <c r="L22" s="6">
+        <v>15</v>
+      </c>
+      <c r="M22" s="6">
+        <v>6</v>
+      </c>
+      <c r="N22" s="6">
+        <v>8</v>
+      </c>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6">
+        <v>1</v>
+      </c>
+      <c r="R22" s="7"/>
+      <c r="S22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="U22" s="7"/>
+      <c r="V22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="W22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="2">
+        <v>67</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K23" s="6">
+        <v>2</v>
+      </c>
+      <c r="L23" s="6">
+        <v>30</v>
+      </c>
+      <c r="M23" s="6">
+        <v>24</v>
+      </c>
+      <c r="N23" s="6">
+        <v>6</v>
+      </c>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T23" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="U23" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="V23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="W23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="2">
+        <v>728</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="6">
+        <v>2</v>
+      </c>
+      <c r="L24" s="6">
+        <v>30</v>
+      </c>
+      <c r="M24" s="6">
+        <v>30</v>
+      </c>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="V24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="W24" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="7">
+        <v>2023</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" s="2">
+        <v>728</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K25" s="6">
+        <v>2</v>
+      </c>
+      <c r="L25" s="6">
+        <v>30</v>
+      </c>
+      <c r="M25" s="6">
+        <v>24</v>
+      </c>
+      <c r="N25" s="6">
+        <v>6</v>
+      </c>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="T25" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="U25" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="V25" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="W25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:Y2" xr:uid="{98DE5E36-27AA-4A14-8D91-698733F7987A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>